<commit_message>
Update et creation des tables de la base de données
</commit_message>
<xml_diff>
--- a/Documents/ListDBStreamFaction.xlsx
+++ b/Documents/ListDBStreamFaction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjetsDevsVSS2019\StreamFaction\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65E42A6D-E22A-4D2C-BE67-D1BE8979AB84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B015B8-0F20-4527-B2ED-E0EBF2A95B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4AF6633-3292-4E52-A099-0D83FCA1AEF0}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{D4AF6633-3292-4E52-A099-0D83FCA1AEF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Status</t>
   </si>
@@ -108,9 +108,6 @@
     <t>usrif_modif_date</t>
   </si>
   <si>
-    <t>sta_id</t>
-  </si>
-  <si>
     <t>Channels</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>sta_logo</t>
   </si>
   <si>
-    <t>Ban_List</t>
-  </si>
-  <si>
     <t>ban_creat_date</t>
   </si>
   <si>
@@ -208,6 +202,30 @@
   </si>
   <si>
     <t>evt_Creat_date</t>
+  </si>
+  <si>
+    <t>Bans</t>
+  </si>
+  <si>
+    <t>Ban_Types</t>
+  </si>
+  <si>
+    <t>bant_id</t>
+  </si>
+  <si>
+    <t>Users_Status</t>
+  </si>
+  <si>
+    <t>usr_sta_create_date</t>
+  </si>
+  <si>
+    <t>usr_sta_modif_date</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>usrsta_ID</t>
   </si>
 </sst>
 </file>
@@ -569,223 +587,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3709734E-F631-451F-87D7-7C5A27FFC76A}">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="2" t="s">
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="H12" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>